<commit_message>
re-calibrated biomass cuttoff; added observed min weight for each species based on length data (Length_SOLACE.rmd) and L-W conversions
</commit_message>
<xml_diff>
--- a/species_params/MesoMizer species params.xlsx
+++ b/species_params/MesoMizer species params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/katherine_baker_utas_edu_au/Documents/Desktop/PhD_Salamanca/RstudioProjects/02_MesoMizer/species_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="820" documentId="8_{83FBC545-D4DB-484A-90C5-15CB6AB9FAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59A1935B-728F-491B-B596-6BB68D433661}"/>
+  <xr:revisionPtr revIDLastSave="827" documentId="8_{83FBC545-D4DB-484A-90C5-15CB6AB9FAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF0CFB26-9F15-445D-98F9-E345A0815FFA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{AC8F4A76-8BA8-430E-AB3A-4F830011832E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AC8F4A76-8BA8-430E-AB3A-4F830011832E}"/>
   </bookViews>
   <sheets>
     <sheet name="Species params" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="173">
   <si>
     <t>Grouping</t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>predator = column</t>
+  </si>
+  <si>
+    <t>Fishbase based on bathylagus antarcticus</t>
   </si>
 </sst>
 </file>
@@ -730,10 +733,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1053,11 +1052,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDE20A8-FF39-42EE-BAEE-B6C1D4AA2AA1}">
-  <dimension ref="A1:AG25"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K25" sqref="K25"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH19" sqref="AH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1077,7 @@
     <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="H1" s="20" t="s">
         <v>77</v>
       </c>
@@ -1116,7 +1115,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1213,8 +1212,14 @@
       <c r="AF2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1252,7 +1257,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1293,7 +1298,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1334,7 +1339,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1366,7 +1371,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1406,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1436,7 +1441,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1474,7 +1479,7 @@
         <v>26.78</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1503,7 +1508,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1575,8 +1580,14 @@
       <c r="Y12">
         <v>81.430000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG12">
+        <v>9.3299999999999998E-3</v>
+      </c>
+      <c r="AH12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1611,7 +1622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1646,7 +1657,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1922,10 +1933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2368AA7B-23E6-450E-954C-5FED4164595D}">
-  <dimension ref="A1:AE25"/>
+  <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,7 +1955,7 @@
     <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G1" s="20" t="s">
         <v>77</v>
       </c>
@@ -1981,7 +1992,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2072,8 +2083,14 @@
       <c r="AD2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2102,7 +2119,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2131,7 +2148,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2160,7 +2177,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2180,7 +2197,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2206,7 +2223,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2229,7 +2246,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2258,7 +2275,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2287,7 +2304,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2319,7 +2336,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2347,8 +2364,11 @@
       <c r="AE12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2368,7 +2388,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2391,7 +2411,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2408,7 +2428,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -5004,7 +5024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDAF294-A978-4E95-B57C-CDEB85ED28A5}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>

</xml_diff>